<commit_message>
db test is completed
</commit_message>
<xml_diff>
--- a/src/test/resources/test-data/Brite-ERP_system.xlsx
+++ b/src/test/resources/test-data/Brite-ERP_system.xlsx
@@ -2912,10 +2912,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:E17"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2"/>
@@ -3214,24 +3214,6 @@
       <c r="E17" s="14">
         <v>43495</v>
       </c>
-    </row>
-    <row r="18" spans="1:5">
-      <c r="E18" s="14"/>
-    </row>
-    <row r="19" spans="1:5">
-      <c r="E19" s="14"/>
-    </row>
-    <row r="20" spans="1:5">
-      <c r="E20" s="14"/>
-    </row>
-    <row r="21" spans="1:5">
-      <c r="E21" s="14"/>
-    </row>
-    <row r="22" spans="1:5">
-      <c r="E22" s="14"/>
-    </row>
-    <row r="23" spans="1:5">
-      <c r="E23" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>